<commit_message>
Actualización schedule task semana 3
</commit_message>
<xml_diff>
--- a/documentos/ciclo1/Fabián Becerra/TASK_Fabián Becerra.xlsx
+++ b/documentos/ciclo1/Fabián Becerra/TASK_Fabián Becerra.xlsx
@@ -117,9 +117,6 @@
     <t>Definir la configuracion control process</t>
   </si>
   <si>
-    <t>Generar listado de tareas de la semana</t>
-  </si>
-  <si>
     <t>Realizar plan de calidad(Definir estándares)</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Inspección detallada de pruebas</t>
+  </si>
+  <si>
+    <t>Generar listado de tareas del ciclo</t>
   </si>
 </sst>
 </file>
@@ -428,36 +428,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -470,13 +476,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -782,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,12 +803,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -817,18 +817,18 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="26"/>
+      <c r="B3" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="28"/>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="30">
         <v>41719</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -851,8 +851,8 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
@@ -866,147 +866,147 @@
       <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="17" t="s">
+      <c r="E7" s="17"/>
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="17" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="19"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="20" t="s">
+      <c r="K8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="20" t="s">
+      <c r="L8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>56</v>
+      <c r="A14" s="25" t="s">
+        <v>55</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="5" t="s">
@@ -1020,7 +1020,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="9">
         <v>2</v>
@@ -1047,7 +1047,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="7"/>
       <c r="C15" s="5" t="s">
         <v>26</v>
@@ -1060,7 +1060,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="9">
         <v>5</v>
@@ -1088,7 +1088,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16"/>
+      <c r="A16" s="31"/>
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
         <v>27</v>
@@ -1101,7 +1101,7 @@
         <v>3.5</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G16" s="9">
         <v>1</v>
@@ -1121,7 +1121,7 @@
         <v>0.5</v>
       </c>
       <c r="L16" s="9">
-        <f t="shared" ref="L16:L17" si="1">K16+L15</f>
+        <f t="shared" ref="L16" si="1">K16+L15</f>
         <v>3.5</v>
       </c>
       <c r="M16" s="9">
@@ -1129,8 +1129,8 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>47</v>
+      <c r="A17" s="25" t="s">
+        <v>46</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="5" t="s">
@@ -1144,7 +1144,7 @@
         <v>4.5</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -1160,12 +1160,19 @@
         <f t="shared" ref="J17:J24" si="2">SUM(I17+J16)</f>
         <v>14.899999999999999</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
+      <c r="K17" s="9">
+        <v>1.4</v>
+      </c>
+      <c r="L17" s="9">
+        <f>K17+L16</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M17" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
         <v>29</v>
@@ -1178,7 +1185,7 @@
         <v>6.5</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -1194,13 +1201,20 @@
         <f t="shared" si="2"/>
         <v>21.5</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
+      <c r="K18" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="L18" s="9">
+        <f>K18+L17</f>
+        <v>6.4</v>
+      </c>
+      <c r="M18" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>48</v>
+      <c r="A19" s="25" t="s">
+        <v>47</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="5" t="s">
@@ -1214,7 +1228,7 @@
         <v>7</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -1230,12 +1244,19 @@
         <f>SUM(I19+J18)</f>
         <v>23.2</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
+      <c r="K19" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="L19" s="9">
+        <f t="shared" ref="L19:L25" si="3">K19+L18</f>
+        <v>6.7</v>
+      </c>
+      <c r="M19" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
         <v>31</v>
@@ -1248,7 +1269,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="9">
         <v>1</v>
@@ -1264,12 +1285,19 @@
         <f t="shared" si="2"/>
         <v>26.5</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="9"/>
+      <c r="K20" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="L20" s="9">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="M20" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
         <v>32</v>
@@ -1282,7 +1310,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G21" s="9">
         <v>1</v>
@@ -1298,15 +1326,22 @@
         <f>SUM(I21+J20)</f>
         <v>27.2</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="9"/>
+      <c r="K21" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="L21" s="9">
+        <f t="shared" si="3"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M21" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="D22" s="8">
         <v>1</v>
@@ -1316,7 +1351,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>
@@ -1332,15 +1367,22 @@
         <f t="shared" si="2"/>
         <v>30.5</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="9"/>
+      <c r="K22" s="9">
+        <v>1</v>
+      </c>
+      <c r="L22" s="9">
+        <f t="shared" si="3"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="M22" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="8">
         <v>0.3</v>
@@ -1350,7 +1392,7 @@
         <v>9.5</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" s="9">
         <v>3</v>
@@ -1366,15 +1408,22 @@
         <f t="shared" si="2"/>
         <v>31.5</v>
       </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="9"/>
+      <c r="K23" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="L23" s="9">
+        <f t="shared" si="3"/>
+        <v>9.6</v>
+      </c>
+      <c r="M23" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="8">
         <v>0.2</v>
@@ -1384,7 +1433,7 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="9">
         <v>2</v>
@@ -1400,15 +1449,22 @@
         <f t="shared" si="2"/>
         <v>32.200000000000003</v>
       </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="6"/>
-      <c r="M24" s="9"/>
+      <c r="K24" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="L24" s="9">
+        <f t="shared" si="3"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M24" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="16"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="8">
         <v>3</v>
@@ -1418,7 +1474,7 @@
         <v>12.7</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G25" s="9">
         <v>5</v>
@@ -1434,17 +1490,24 @@
         <f>SUM(I25+J24)</f>
         <v>42.1</v>
       </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="K25" s="9">
+        <v>2.4</v>
+      </c>
+      <c r="L25" s="9">
+        <f t="shared" si="3"/>
+        <v>12.1</v>
+      </c>
+      <c r="M25" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" s="8">
         <v>2</v>
@@ -1454,7 +1517,7 @@
         <v>14.7</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G26" s="9">
         <v>1</v>
@@ -1467,20 +1530,20 @@
         <v>6.6</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" ref="J26:J35" si="3">SUM(I26+J25)</f>
+        <f t="shared" ref="J26:J35" si="4">SUM(I26+J25)</f>
         <v>48.7</v>
       </c>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="6"/>
+      <c r="M26" s="9"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>50</v>
+      <c r="A27" s="25" t="s">
+        <v>49</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="8">
         <v>1</v>
@@ -1490,7 +1553,7 @@
         <v>15.7</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" s="9">
         <v>2</v>
@@ -1503,18 +1566,18 @@
         <v>3.3</v>
       </c>
       <c r="J27" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
-      <c r="M27" s="6"/>
+      <c r="M27" s="9"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D28" s="8">
         <v>0.5</v>
@@ -1524,7 +1587,7 @@
         <v>16.2</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="9">
         <v>1</v>
@@ -1537,18 +1600,18 @@
         <v>1.7</v>
       </c>
       <c r="J28" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>53.7</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="6"/>
+      <c r="M28" s="9"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D29" s="8">
         <v>0.5</v>
@@ -1558,7 +1621,7 @@
         <v>16.7</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29" s="9">
         <v>0.7</v>
@@ -1571,20 +1634,20 @@
         <v>1.7</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>55.400000000000006</v>
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
+      <c r="M29" s="9"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>51</v>
+      <c r="A30" s="25" t="s">
+        <v>50</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="8">
         <v>3.5</v>
@@ -1594,7 +1657,7 @@
         <v>20.2</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G30" s="9">
         <v>3</v>
@@ -1607,18 +1670,18 @@
         <v>11.6</v>
       </c>
       <c r="J30" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
+      <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="8">
         <v>1</v>
@@ -1637,18 +1700,18 @@
         <v>3.3</v>
       </c>
       <c r="J31" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70.3</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="M31" s="9"/>
     </row>
     <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="8">
         <v>0.5</v>
@@ -1658,7 +1721,7 @@
         <v>21.7</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G32" s="9">
         <v>0.7</v>
@@ -1671,7 +1734,7 @@
         <v>1.7</v>
       </c>
       <c r="J32" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72</v>
       </c>
       <c r="K32" s="6"/>
@@ -1679,10 +1742,10 @@
       <c r="M32" s="6"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="7"/>
       <c r="C33" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="8">
         <v>5</v>
@@ -1692,7 +1755,7 @@
         <v>26.7</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G33" s="9">
         <v>646</v>
@@ -1705,7 +1768,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="J33" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88.6</v>
       </c>
       <c r="K33" s="6"/>
@@ -1714,11 +1777,11 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D34" s="8">
         <v>1</v>
@@ -1728,7 +1791,7 @@
         <v>27.7</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" s="9">
         <v>10</v>
@@ -1741,7 +1804,7 @@
         <v>3.3</v>
       </c>
       <c r="J34" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.899999999999991</v>
       </c>
       <c r="K34" s="6"/>
@@ -1749,12 +1812,12 @@
       <c r="M34" s="6"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15" t="s">
-        <v>53</v>
+      <c r="A35" s="25" t="s">
+        <v>52</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D35" s="8">
         <v>1</v>
@@ -1764,7 +1827,7 @@
         <v>28.7</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G35" s="9">
         <v>5</v>
@@ -1777,7 +1840,7 @@
         <v>3.3</v>
       </c>
       <c r="J35" s="9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>95.199999999999989</v>
       </c>
       <c r="K35" s="6"/>
@@ -1785,10 +1848,10 @@
       <c r="M35" s="6"/>
     </row>
     <row r="36" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D36" s="8">
         <v>1.5</v>
@@ -1798,7 +1861,7 @@
         <v>30.2</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G36" s="9">
         <v>5</v>
@@ -1819,31 +1882,12 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="8">
-        <f t="shared" ref="D37" si="4">SUM(D14:D36)</f>
+        <f t="shared" ref="D37" si="5">SUM(D14:D36)</f>
         <v>30.2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="K7:M7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="F8:F13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E3:G3"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="F7:J7"/>
     <mergeCell ref="J8:J13"/>
@@ -1855,6 +1899,25 @@
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="A27:A29"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E8:E13"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="K7:M7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="F8:F13"/>
+    <mergeCell ref="G8:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>